<commit_message>
Adjust PoFDCtAE to meet changes in demand with exports
</commit_message>
<xml_diff>
--- a/InputData/fuels/PoFDCtAE/Perc of Fuel Demand Changes that Affect Exports.xlsx
+++ b/InputData/fuels/PoFDCtAE/Perc of Fuel Demand Changes that Affect Exports.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\Dropbox (Energy InNovation)\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-virginia\InputData\fuels\PoFDCtAE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190E0567-D228-475F-AE92-CB99F12E58B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2055" yWindow="1065" windowWidth="23535" windowHeight="16185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2055" yWindow="1065" windowWidth="23535" windowHeight="16185"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Data from BFPIaE" sheetId="3" r:id="rId2"/>
     <sheet name="PoFDCtAE" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -340,7 +339,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000E+00"/>
   </numFmts>
@@ -787,22 +786,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="87.5703125" customWidth="1"/>
+    <col min="2" max="2" width="87.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -810,223 +809,223 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B12" s="26" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B13" s="27" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A47" s="32" t="s">
         <v>92</v>
       </c>
       <c r="B47" s="33"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A57" s="14" t="s">
         <v>53</v>
       </c>
@@ -1038,87 +1037,87 @@
       <c r="G57" s="15"/>
       <c r="H57" s="15"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>62</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B9" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B7" r:id="rId1"/>
+    <hyperlink ref="B8" r:id="rId2"/>
+    <hyperlink ref="B9" r:id="rId3"/>
+    <hyperlink ref="B10" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -1126,26 +1125,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="44.140625" customWidth="1"/>
-    <col min="2" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="100.7109375" customWidth="1"/>
+    <col min="1" max="1" width="44.1328125" customWidth="1"/>
+    <col min="2" max="5" width="15.3984375" customWidth="1"/>
+    <col min="6" max="6" width="12.86328125" customWidth="1"/>
+    <col min="7" max="7" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="100.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="14" t="s">
         <v>70</v>
       </c>
@@ -1158,7 +1157,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="18" t="s">
         <v>71</v>
       </c>
@@ -1181,7 +1180,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>32</v>
       </c>
@@ -1194,7 +1193,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
@@ -1219,7 +1218,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>34</v>
       </c>
@@ -1244,7 +1243,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>78</v>
       </c>
@@ -1269,7 +1268,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="7" t="s">
         <v>36</v>
       </c>
@@ -1283,7 +1282,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="7" t="s">
         <v>37</v>
       </c>
@@ -1294,7 +1293,7 @@
       <c r="F9" s="23"/>
       <c r="G9" s="30"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="7" t="s">
         <v>38</v>
       </c>
@@ -1305,7 +1304,7 @@
       <c r="F10" s="23"/>
       <c r="G10" s="30"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>39</v>
       </c>
@@ -1327,7 +1326,7 @@
       </c>
       <c r="G11" s="30"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="28" t="s">
         <v>40</v>
       </c>
@@ -1349,7 +1348,7 @@
       </c>
       <c r="G12" s="30"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="28" t="s">
         <v>41</v>
       </c>
@@ -1371,7 +1370,7 @@
       </c>
       <c r="G13" s="30"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>42</v>
       </c>
@@ -1393,7 +1392,7 @@
       </c>
       <c r="G14" s="30"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>43</v>
       </c>
@@ -1415,7 +1414,7 @@
       </c>
       <c r="G15" s="30"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="28" t="s">
         <v>44</v>
       </c>
@@ -1437,7 +1436,7 @@
       </c>
       <c r="G16" s="30"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="7" t="s">
         <v>45</v>
       </c>
@@ -1448,7 +1447,7 @@
       <c r="F17" s="23"/>
       <c r="G17" s="30"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="7" t="s">
         <v>46</v>
       </c>
@@ -1459,7 +1458,7 @@
       <c r="F18" s="23"/>
       <c r="G18" s="30"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>47</v>
       </c>
@@ -1481,7 +1480,7 @@
       </c>
       <c r="G19" s="30"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>48</v>
       </c>
@@ -1503,7 +1502,7 @@
       </c>
       <c r="G20" s="30"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="28" t="s">
         <v>49</v>
       </c>
@@ -1525,7 +1524,7 @@
       </c>
       <c r="G21" s="30"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="28" t="s">
         <v>50</v>
       </c>
@@ -1547,7 +1546,7 @@
       </c>
       <c r="G22" s="30"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="6" t="s">
         <v>51</v>
       </c>
@@ -1569,7 +1568,7 @@
       </c>
       <c r="G23" s="30"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="6" t="s">
         <v>52</v>
       </c>
@@ -1597,7 +1596,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1607,16 +1606,16 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" customWidth="1"/>
-    <col min="2" max="22" width="16.5703125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="36.73046875" customWidth="1"/>
+    <col min="2" max="22" width="16.59765625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>69</v>
       </c>
@@ -1684,7 +1683,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>32</v>
       </c>
@@ -1752,7 +1751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>33</v>
       </c>
@@ -1760,8 +1759,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="31">
-        <f>'Data from BFPIaE'!D5/'Data from BFPIaE'!B5</f>
-        <v>0.14686588977933832</v>
+        <v>1</v>
       </c>
       <c r="D3" s="8">
         <v>0</v>
@@ -1821,7 +1819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>34</v>
       </c>
@@ -1832,8 +1830,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="31">
-        <f>'Data from BFPIaE'!D6/'Data from BFPIaE'!B6</f>
-        <v>0.15500746052469119</v>
+        <v>1</v>
       </c>
       <c r="E4" s="8">
         <v>0</v>
@@ -1890,7 +1887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>35</v>
       </c>
@@ -1959,7 +1956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
         <v>36</v>
       </c>
@@ -2027,7 +2024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A7" s="7" t="s">
         <v>37</v>
       </c>
@@ -2095,7 +2092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A8" s="7" t="s">
         <v>38</v>
       </c>
@@ -2163,7 +2160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
@@ -2189,8 +2186,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="31">
-        <f>'Data from BFPIaE'!D11/'Data from BFPIaE'!B11</f>
-        <v>0.68036965837987495</v>
+        <v>1</v>
       </c>
       <c r="J9" s="8">
         <v>0</v>
@@ -2232,7 +2228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>40</v>
       </c>
@@ -2261,8 +2257,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="12">
-        <f>'Data from BFPIaE'!D12/SUM('Data from BFPIaE'!D12:E12)</f>
-        <v>7.2806513229885905E-2</v>
+        <v>1</v>
       </c>
       <c r="K10" s="8">
         <v>0</v>
@@ -2287,7 +2282,7 @@
       </c>
       <c r="R10" s="13">
         <f>1-J10</f>
-        <v>0.92719348677011415</v>
+        <v>0</v>
       </c>
       <c r="S10" s="8">
         <v>0</v>
@@ -2302,7 +2297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>41</v>
       </c>
@@ -2334,8 +2329,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="12">
-        <f>'Data from BFPIaE'!D13/SUM('Data from BFPIaE'!D13:E13)</f>
-        <v>0.26002912808189416</v>
+        <v>1</v>
       </c>
       <c r="L11" s="8">
         <v>0</v>
@@ -2357,7 +2351,7 @@
       </c>
       <c r="R11" s="13">
         <f>1-K11</f>
-        <v>0.73997087191810584</v>
+        <v>0</v>
       </c>
       <c r="S11" s="8">
         <v>0</v>
@@ -2372,7 +2366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>42</v>
       </c>
@@ -2407,8 +2401,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="31">
-        <f>'Data from BFPIaE'!D14/'Data from BFPIaE'!B14</f>
-        <v>0.10491259896601664</v>
+        <v>1</v>
       </c>
       <c r="M12" s="8">
         <v>0</v>
@@ -2441,7 +2434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>43</v>
       </c>
@@ -2479,8 +2472,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="31">
-        <f>'Data from BFPIaE'!D15/'Data from BFPIaE'!B15</f>
-        <v>7.0542950086431883E-2</v>
+        <v>1</v>
       </c>
       <c r="N13" s="8">
         <v>0</v>
@@ -2510,7 +2502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>44</v>
       </c>
@@ -2551,8 +2543,7 @@
         <v>0</v>
       </c>
       <c r="N14" s="12">
-        <f>'Data from BFPIaE'!D16/SUM('Data from BFPIaE'!D16:E16)</f>
-        <v>9.9755024140854479E-2</v>
+        <v>1</v>
       </c>
       <c r="O14" s="11">
         <v>0</v>
@@ -2565,7 +2556,7 @@
       </c>
       <c r="R14" s="13">
         <f>1-N14</f>
-        <v>0.90024497585914554</v>
+        <v>0</v>
       </c>
       <c r="S14" s="8">
         <v>0</v>
@@ -2580,7 +2571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A15" s="7" t="s">
         <v>45</v>
       </c>
@@ -2648,7 +2639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A16" s="7" t="s">
         <v>46</v>
       </c>
@@ -2716,7 +2707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
         <v>47</v>
       </c>
@@ -2785,7 +2776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>48</v>
       </c>
@@ -2853,7 +2844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>49</v>
       </c>
@@ -2907,11 +2898,10 @@
       </c>
       <c r="R19" s="13">
         <f>1-S19</f>
-        <v>0.49404181432894001</v>
+        <v>0</v>
       </c>
       <c r="S19" s="12">
-        <f>'Data from BFPIaE'!D21/SUM('Data from BFPIaE'!D21:E21)</f>
-        <v>0.50595818567105999</v>
+        <v>1</v>
       </c>
       <c r="T19" s="8">
         <v>0</v>
@@ -2923,7 +2913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>50</v>
       </c>
@@ -2977,14 +2967,13 @@
       </c>
       <c r="R20" s="13">
         <f>1-T20</f>
-        <v>0.57774176716224113</v>
+        <v>0</v>
       </c>
       <c r="S20" s="8">
         <v>0</v>
       </c>
       <c r="T20" s="12">
-        <f>'Data from BFPIaE'!D22/SUM('Data from BFPIaE'!D22:E22)</f>
-        <v>0.42225823283775882</v>
+        <v>1</v>
       </c>
       <c r="U20" s="8">
         <v>0</v>
@@ -2993,7 +2982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>51</v>
       </c>
@@ -3062,7 +3051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
UT edit to PoFDCtAE
</commit_message>
<xml_diff>
--- a/InputData/fuels/PoFDCtAE/Perc of Fuel Demand Changes that Affect Exports.xlsx
+++ b/InputData/fuels/PoFDCtAE/Perc of Fuel Demand Changes that Affect Exports.xlsx
@@ -5,36 +5,27 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-virginia\InputData\fuels\PoFDCtAE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-texas\InputData\fuels\PoFDCtAE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2055" yWindow="1065" windowWidth="23535" windowHeight="16185"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6585"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="Data from BFPIaE" sheetId="3" r:id="rId2"/>
-    <sheet name="PoFDCtAE" sheetId="2" r:id="rId3"/>
+    <sheet name="PoFDCtAE" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="85">
   <si>
     <t>PoFDCtAE Percentage of Fuel Demand Change that Alters Exports</t>
   </si>
@@ -105,6 +96,9 @@
     <t>This variable allows you to specify this behavior for a given country.</t>
   </si>
   <si>
+    <t>a great deal of capacity to increase or decrease its own production</t>
+  </si>
+  <si>
     <t>Saudi Arabia is a major crude oil exporter.  Saudi Arabia's cost to produce</t>
   </si>
   <si>
@@ -132,6 +126,33 @@
     <t>rather than changes in production or imports.</t>
   </si>
   <si>
+    <t>Example 1: The United States</t>
+  </si>
+  <si>
+    <t>Example 2: Saudi Arabia</t>
+  </si>
+  <si>
+    <t>The following examples may help you set this variable wisely:</t>
+  </si>
+  <si>
+    <t>The United States is a major exporter of oil.  The U.S. has</t>
+  </si>
+  <si>
+    <t>to meet demand.  Its oil is not exceptionally cheap to produce and</t>
+  </si>
+  <si>
+    <t>comes in around the global marginal price, accounting for shipping costs.</t>
+  </si>
+  <si>
+    <t>If the U.S. could export more oil profitably, it would already be doing so.</t>
+  </si>
+  <si>
+    <t>Changes in domestic oil demand are likely to be met with changes</t>
+  </si>
+  <si>
+    <t>in production and imports.</t>
+  </si>
+  <si>
     <t>electricity (not used in this variable)</t>
   </si>
   <si>
@@ -246,103 +267,25 @@
     <t>Percentage Change in Demand that Alters Exports (dimensionless) - From type (below)  / To type (right)</t>
   </si>
   <si>
-    <t>Converted to BTU</t>
-  </si>
-  <si>
-    <t>Fuel</t>
-  </si>
-  <si>
-    <t>Production</t>
-  </si>
-  <si>
-    <t>Imports</t>
-  </si>
-  <si>
-    <t>Exports</t>
-  </si>
-  <si>
-    <t>Domestic Use</t>
-  </si>
-  <si>
-    <t>Unit</t>
-  </si>
-  <si>
-    <t>BTU</t>
-  </si>
-  <si>
-    <t>uranium</t>
-  </si>
-  <si>
-    <t>Start Year Data</t>
-  </si>
-  <si>
     <t>Overall Approach and Assumptions</t>
   </si>
   <si>
-    <t>Apportioning Secondary Product Changes to That Product vs. Crude Oil</t>
-  </si>
-  <si>
-    <t>see variable fuels/BFPIaE</t>
-  </si>
-  <si>
-    <t>We estimate the response to a drop in domestic use of a secondary petroleum product by observing how large</t>
-  </si>
-  <si>
-    <t>the export market for that fuel is, versus the domestic use market.  If the fuel's exports are a far larger share</t>
-  </si>
-  <si>
-    <t>of the total outflows (exports + use) than use is, we assume the export market for that fuel can more easily</t>
-  </si>
-  <si>
-    <t>absorb the drop in domestic production.  Where a fuel is more commonly produced for domestic use (where</t>
-  </si>
-  <si>
-    <t>use has a larger share than exports of the total outflows), we assume less of that fuel will be produced, and</t>
-  </si>
-  <si>
-    <t>more crude will be exported instead.</t>
-  </si>
-  <si>
-    <t>Reasoning</t>
-  </si>
-  <si>
-    <t>The following example may help you set this variable wisely:</t>
-  </si>
-  <si>
-    <t>Example 1: Saudi Arabia</t>
-  </si>
-  <si>
-    <t>United States Settings</t>
-  </si>
-  <si>
-    <t>Based on consultation with oil market experts at Rapidian Energy and Wood Mackenzie,</t>
-  </si>
-  <si>
-    <t>in a high electrification scenario), and the difference would be made up by increased exports,</t>
-  </si>
-  <si>
-    <t>similar to the Saudi Arabia example above.</t>
-  </si>
-  <si>
-    <t>day exports / present day production), which should roughly express how important the export market</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> for that fuel for U.S. producers.</t>
-  </si>
-  <si>
-    <t>we believe U.S. oil production would be relatively unaffected by a drop in U.S. demand (for instance,</t>
-  </si>
-  <si>
-    <t>For fuels other than crude oil and petroleum products, we use settings calculated as (present</t>
+    <t>a region with non-zero changes in exports in response to chagnes in production,</t>
+  </si>
+  <si>
+    <t>https://saudiarabia.energypolicy.solutions</t>
+  </si>
+  <si>
+    <t>For an example of how to calculate the input data for this variable in</t>
+  </si>
+  <si>
+    <t>see this variable in the Saudi Arabia version of the Energy Policy Simulator:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000E+00"/>
-  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -376,7 +319,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -397,25 +340,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -433,7 +358,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -460,52 +385,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -787,9 +673,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H74"/>
+  <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -805,7 +693,7 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="14" t="s">
         <v>80</v>
       </c>
     </row>
@@ -844,273 +732,336 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B12" s="26" t="s">
-        <v>81</v>
-      </c>
-    </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B13" s="27" t="s">
-        <v>82</v>
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" s="1" t="s">
-        <v>8</v>
+      <c r="B16" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>9</v>
+      <c r="B17" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B19" t="s">
-        <v>13</v>
+      <c r="B18" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B20" t="s">
-        <v>11</v>
+      <c r="A20" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B21" t="s">
-        <v>12</v>
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A33" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A36" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A42" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A47" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="B47" s="33"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
-        <v>93</v>
-      </c>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>98</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>94</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="18"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>95</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="18"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="C52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="18"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
-        <v>99</v>
-      </c>
+      <c r="A53" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B53" s="13"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>96</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="18"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>97</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="18"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>66</v>
+      </c>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="18"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A57" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B57" s="15"/>
-      <c r="C57" s="15"/>
-      <c r="D57" s="15"/>
-      <c r="E57" s="15"/>
-      <c r="F57" s="15"/>
-      <c r="G57" s="15"/>
-      <c r="H57" s="15"/>
+      <c r="A57" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A67" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A72" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A73" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A74" t="s">
-        <v>62</v>
-      </c>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A72" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B72" s="16"/>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A73" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B73" s="16"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A74" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B74" s="16"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A75" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B75" s="16"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1118,484 +1069,14 @@
     <hyperlink ref="B8" r:id="rId2"/>
     <hyperlink ref="B9" r:id="rId3"/>
     <hyperlink ref="B10" r:id="rId4"/>
+    <hyperlink ref="A75" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="44.1328125" customWidth="1"/>
-    <col min="2" max="5" width="15.3984375" customWidth="1"/>
-    <col min="6" max="6" width="12.86328125" customWidth="1"/>
-    <col min="7" max="7" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="100.73046875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A2" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="17"/>
-      <c r="H2" s="29" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="H3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="23"/>
-      <c r="H4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="24">
-        <v>1.2994850819999496E+16</v>
-      </c>
-      <c r="C5" s="24">
-        <v>121838241144116.98</v>
-      </c>
-      <c r="D5" s="24">
-        <v>1908500328228990.3</v>
-      </c>
-      <c r="E5" s="22">
-        <f t="shared" ref="E5:E24" si="0">B5+C5-D5</f>
-        <v>1.1208188732914622E+16</v>
-      </c>
-      <c r="F5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G5" s="30"/>
-      <c r="H5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="24">
-        <v>3.3449389999999996E+16</v>
-      </c>
-      <c r="C6" s="24">
-        <v>2724850000000000</v>
-      </c>
-      <c r="D6" s="24">
-        <v>5184905000000000</v>
-      </c>
-      <c r="E6" s="22">
-        <f t="shared" si="0"/>
-        <v>3.0989335E+16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>77</v>
-      </c>
-      <c r="G6" s="30"/>
-      <c r="H6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A7" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" s="24">
-        <v>534894468127151.31</v>
-      </c>
-      <c r="C7" s="24">
-        <v>7200000000000000</v>
-      </c>
-      <c r="D7" s="24">
-        <v>0</v>
-      </c>
-      <c r="E7" s="22">
-        <f t="shared" si="0"/>
-        <v>7734894468127151</v>
-      </c>
-      <c r="F7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G7" s="30"/>
-      <c r="H7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A8" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="30"/>
-      <c r="H8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A9" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="30"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A10" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="30"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A11" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="24">
-        <v>127054236057268.86</v>
-      </c>
-      <c r="C11" s="24">
-        <v>3835846580378.2954</v>
-      </c>
-      <c r="D11" s="24">
-        <v>86443847182000</v>
-      </c>
-      <c r="E11" s="22">
-        <f t="shared" si="0"/>
-        <v>44446235455647.156</v>
-      </c>
-      <c r="F11" t="s">
-        <v>77</v>
-      </c>
-      <c r="G11" s="30"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A12" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="24">
-        <v>2.345837516236748E+16</v>
-      </c>
-      <c r="C12" s="24">
-        <v>65450425688886.055</v>
-      </c>
-      <c r="D12" s="24">
-        <v>1712687718894354.5</v>
-      </c>
-      <c r="E12" s="22">
-        <f t="shared" si="0"/>
-        <v>2.1811137869162012E+16</v>
-      </c>
-      <c r="F12" t="s">
-        <v>77</v>
-      </c>
-      <c r="G12" s="30"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A13" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="24">
-        <v>1.3635229972917368E+16</v>
-      </c>
-      <c r="C13" s="24">
-        <v>351737454255556.31</v>
-      </c>
-      <c r="D13" s="24">
-        <v>3637018944597630</v>
-      </c>
-      <c r="E13" s="22">
-        <f t="shared" si="0"/>
-        <v>1.0349948482575294E+16</v>
-      </c>
-      <c r="F13" t="s">
-        <v>77</v>
-      </c>
-      <c r="G13" s="30"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A14" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="24">
-        <v>1561489169872463.5</v>
-      </c>
-      <c r="C14" s="24">
-        <v>8008300000911.835</v>
-      </c>
-      <c r="D14" s="24">
-        <v>163819887068608</v>
-      </c>
-      <c r="E14" s="22">
-        <f t="shared" si="0"/>
-        <v>1405677582804767.3</v>
-      </c>
-      <c r="F14" t="s">
-        <v>77</v>
-      </c>
-      <c r="G14" s="30"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A15" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="24">
-        <v>209619113794859.22</v>
-      </c>
-      <c r="C15" s="24">
-        <v>81719279513151.391</v>
-      </c>
-      <c r="D15" s="24">
-        <v>14787150681592.84</v>
-      </c>
-      <c r="E15" s="22">
-        <f t="shared" si="0"/>
-        <v>276551242626417.78</v>
-      </c>
-      <c r="F15" t="s">
-        <v>77</v>
-      </c>
-      <c r="G15" s="30"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A16" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="24">
-        <v>4515477159886859</v>
-      </c>
-      <c r="C16" s="24">
-        <v>371817123993646.19</v>
-      </c>
-      <c r="D16" s="24">
-        <v>487532159271959.88</v>
-      </c>
-      <c r="E16" s="22">
-        <f t="shared" si="0"/>
-        <v>4399762124608545</v>
-      </c>
-      <c r="F16" t="s">
-        <v>77</v>
-      </c>
-      <c r="G16" s="30"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A17" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="30"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="30"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="24">
-        <v>859050369312946.75</v>
-      </c>
-      <c r="C19" s="24">
-        <v>0</v>
-      </c>
-      <c r="D19" s="24">
-        <v>0</v>
-      </c>
-      <c r="E19" s="22">
-        <f t="shared" si="0"/>
-        <v>859050369312946.75</v>
-      </c>
-      <c r="F19" t="s">
-        <v>77</v>
-      </c>
-      <c r="G19" s="30"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A20" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="24">
-        <v>2.4934676413517276E+16</v>
-      </c>
-      <c r="C20" s="24">
-        <v>1.4838296942851536E+16</v>
-      </c>
-      <c r="D20" s="24">
-        <v>2994708229987662</v>
-      </c>
-      <c r="E20" s="22">
-        <f t="shared" si="0"/>
-        <v>3.6778265126381152E+16</v>
-      </c>
-      <c r="F20" t="s">
-        <v>77</v>
-      </c>
-      <c r="G20" s="30"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A21" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="24">
-        <v>1250687800589910.5</v>
-      </c>
-      <c r="C21" s="24">
-        <v>476589424280788.31</v>
-      </c>
-      <c r="D21" s="24">
-        <v>873930050846522.25</v>
-      </c>
-      <c r="E21" s="22">
-        <f t="shared" si="0"/>
-        <v>853347174024176.5</v>
-      </c>
-      <c r="F21" t="s">
-        <v>77</v>
-      </c>
-      <c r="G21" s="30"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A22" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="24">
-        <v>4084904971604980.5</v>
-      </c>
-      <c r="C22" s="24">
-        <v>243930593817797.94</v>
-      </c>
-      <c r="D22" s="24">
-        <v>1827886456100663</v>
-      </c>
-      <c r="E22" s="22">
-        <f t="shared" si="0"/>
-        <v>2500949109322115.5</v>
-      </c>
-      <c r="F22" t="s">
-        <v>77</v>
-      </c>
-      <c r="G22" s="30"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A23" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="24">
-        <v>1730154785433083.3</v>
-      </c>
-      <c r="C23" s="24">
-        <v>0</v>
-      </c>
-      <c r="D23" s="24">
-        <v>0</v>
-      </c>
-      <c r="E23" s="22">
-        <f t="shared" si="0"/>
-        <v>1730154785433083.3</v>
-      </c>
-      <c r="F23" t="s">
-        <v>77</v>
-      </c>
-      <c r="G23" s="30"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A24" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" s="24">
-        <v>8746500000000000</v>
-      </c>
-      <c r="C24" s="24">
-        <v>0</v>
-      </c>
-      <c r="D24" s="24">
-        <v>0</v>
-      </c>
-      <c r="E24" s="22">
-        <f t="shared" si="0"/>
-        <v>8746500000000000</v>
-      </c>
-      <c r="F24" t="s">
-        <v>77</v>
-      </c>
-      <c r="G24" s="30"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
@@ -1606,7 +1087,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U20" sqref="U20"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1617,75 +1098,75 @@
   <sheetData>
     <row r="1" spans="1:22" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="Q1" s="10" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="R1" s="10" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="S1" s="10" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="T1" s="10" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="U1" s="10" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="V1" s="10" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B2" s="11">
         <v>0</v>
@@ -1753,13 +1234,13 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B3" s="11">
         <v>0</v>
       </c>
-      <c r="C3" s="31">
-        <v>1</v>
+      <c r="C3" s="8">
+        <v>0</v>
       </c>
       <c r="D3" s="8">
         <v>0</v>
@@ -1821,7 +1302,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B4" s="11">
         <v>0</v>
@@ -1829,8 +1310,8 @@
       <c r="C4" s="8">
         <v>0</v>
       </c>
-      <c r="D4" s="31">
-        <v>1</v>
+      <c r="D4" s="8">
+        <v>0</v>
       </c>
       <c r="E4" s="8">
         <v>0</v>
@@ -1889,7 +1370,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B5" s="11">
         <v>0</v>
@@ -1900,8 +1381,7 @@
       <c r="D5" s="8">
         <v>0</v>
       </c>
-      <c r="E5" s="31">
-        <f>'Data from BFPIaE'!D7/'Data from BFPIaE'!B7</f>
+      <c r="E5" s="8">
         <v>0</v>
       </c>
       <c r="F5" s="11">
@@ -1958,7 +1438,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B6" s="11">
         <v>0</v>
@@ -2026,7 +1506,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A7" s="7" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B7" s="11">
         <v>0</v>
@@ -2094,7 +1574,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A8" s="7" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B8" s="11">
         <v>0</v>
@@ -2162,7 +1642,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B9" s="11">
         <v>0</v>
@@ -2185,8 +1665,8 @@
       <c r="H9" s="11">
         <v>0</v>
       </c>
-      <c r="I9" s="31">
-        <v>1</v>
+      <c r="I9" s="8">
+        <v>0</v>
       </c>
       <c r="J9" s="8">
         <v>0</v>
@@ -2230,7 +1710,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B10" s="11">
         <v>0</v>
@@ -2256,8 +1736,8 @@
       <c r="I10" s="8">
         <v>0</v>
       </c>
-      <c r="J10" s="12">
-        <v>1</v>
+      <c r="J10" s="8">
+        <v>0</v>
       </c>
       <c r="K10" s="8">
         <v>0</v>
@@ -2280,8 +1760,7 @@
       <c r="Q10" s="8">
         <v>0</v>
       </c>
-      <c r="R10" s="13">
-        <f>1-J10</f>
+      <c r="R10" s="8">
         <v>0</v>
       </c>
       <c r="S10" s="8">
@@ -2299,7 +1778,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B11" s="11">
         <v>0</v>
@@ -2328,8 +1807,8 @@
       <c r="J11" s="8">
         <v>0</v>
       </c>
-      <c r="K11" s="12">
-        <v>1</v>
+      <c r="K11" s="8">
+        <v>0</v>
       </c>
       <c r="L11" s="8">
         <v>0</v>
@@ -2349,8 +1828,7 @@
       <c r="Q11" s="8">
         <v>0</v>
       </c>
-      <c r="R11" s="13">
-        <f>1-K11</f>
+      <c r="R11" s="8">
         <v>0</v>
       </c>
       <c r="S11" s="8">
@@ -2368,7 +1846,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B12" s="11">
         <v>0</v>
@@ -2400,8 +1878,8 @@
       <c r="K12" s="8">
         <v>0</v>
       </c>
-      <c r="L12" s="31">
-        <v>1</v>
+      <c r="L12" s="8">
+        <v>0</v>
       </c>
       <c r="M12" s="8">
         <v>0</v>
@@ -2436,7 +1914,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B13" s="11">
         <v>0</v>
@@ -2471,8 +1949,8 @@
       <c r="L13" s="8">
         <v>0</v>
       </c>
-      <c r="M13" s="31">
-        <v>1</v>
+      <c r="M13" s="8">
+        <v>0</v>
       </c>
       <c r="N13" s="8">
         <v>0</v>
@@ -2504,7 +1982,7 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B14" s="11">
         <v>0</v>
@@ -2542,8 +2020,8 @@
       <c r="M14" s="8">
         <v>0</v>
       </c>
-      <c r="N14" s="12">
-        <v>1</v>
+      <c r="N14" s="8">
+        <v>0</v>
       </c>
       <c r="O14" s="11">
         <v>0</v>
@@ -2554,8 +2032,7 @@
       <c r="Q14" s="8">
         <v>0</v>
       </c>
-      <c r="R14" s="13">
-        <f>1-N14</f>
+      <c r="R14" s="8">
         <v>0</v>
       </c>
       <c r="S14" s="8">
@@ -2573,7 +2050,7 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A15" s="7" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B15" s="11">
         <v>0</v>
@@ -2641,7 +2118,7 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A16" s="7" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B16" s="11">
         <v>0</v>
@@ -2709,7 +2186,7 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="B17" s="11">
         <v>0</v>
@@ -2756,8 +2233,7 @@
       <c r="P17" s="11">
         <v>0</v>
       </c>
-      <c r="Q17" s="31">
-        <f>'Data from BFPIaE'!D19/'Data from BFPIaE'!B19</f>
+      <c r="Q17" s="8">
         <v>0</v>
       </c>
       <c r="R17" s="8">
@@ -2778,7 +2254,7 @@
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B18" s="11">
         <v>0</v>
@@ -2828,8 +2304,8 @@
       <c r="Q18" s="8">
         <v>0</v>
       </c>
-      <c r="R18" s="12">
-        <v>1</v>
+      <c r="R18" s="8">
+        <v>0</v>
       </c>
       <c r="S18" s="8">
         <v>0</v>
@@ -2846,7 +2322,7 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B19" s="11">
         <v>0</v>
@@ -2896,12 +2372,11 @@
       <c r="Q19" s="8">
         <v>0</v>
       </c>
-      <c r="R19" s="13">
-        <f>1-S19</f>
-        <v>0</v>
-      </c>
-      <c r="S19" s="12">
-        <v>1</v>
+      <c r="R19" s="8">
+        <v>0</v>
+      </c>
+      <c r="S19" s="8">
+        <v>0</v>
       </c>
       <c r="T19" s="8">
         <v>0</v>
@@ -2915,7 +2390,7 @@
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B20" s="11">
         <v>0</v>
@@ -2965,15 +2440,14 @@
       <c r="Q20" s="8">
         <v>0</v>
       </c>
-      <c r="R20" s="13">
-        <f>1-T20</f>
+      <c r="R20" s="8">
         <v>0</v>
       </c>
       <c r="S20" s="8">
         <v>0</v>
       </c>
-      <c r="T20" s="12">
-        <v>1</v>
+      <c r="T20" s="8">
+        <v>0</v>
       </c>
       <c r="U20" s="8">
         <v>0</v>
@@ -2984,7 +2458,7 @@
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="B21" s="11">
         <v>0</v>
@@ -3043,8 +2517,7 @@
       <c r="T21" s="8">
         <v>0</v>
       </c>
-      <c r="U21" s="31">
-        <f>'Data from BFPIaE'!D23/'Data from BFPIaE'!B23</f>
+      <c r="U21" s="8">
         <v>0</v>
       </c>
       <c r="V21" s="8">
@@ -3053,7 +2526,7 @@
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B22" s="11">
         <v>0</v>
@@ -3115,8 +2588,7 @@
       <c r="U22" s="8">
         <v>0</v>
       </c>
-      <c r="V22" s="31">
-        <f>'Data from BFPIaE'!D24/'Data from BFPIaE'!B24</f>
+      <c r="V22" s="8">
         <v>0</v>
       </c>
     </row>

</xml_diff>